<commit_message>
Added WING, YOU, KLAC, SPLK, WDAY, and HUBS models
</commit_message>
<xml_diff>
--- a/Consumer/Ulta Beauty.xlsx
+++ b/Consumer/Ulta Beauty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Value/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Consumer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4D3267-8A68-B541-BD9A-EB3F5F900327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120CBD37-591F-5E4B-AA54-2654954FAD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="500" windowWidth="27900" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="500" windowWidth="27900" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -972,6 +972,18 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -983,18 +995,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1085,10 +1085,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.4971767982785005E-2"/>
-          <c:y val="0.15340781139999113"/>
-          <c:w val="0.84149134090981581"/>
-          <c:h val="0.71317857950620589"/>
+          <c:x val="8.3024905370712457E-2"/>
+          <c:y val="0.12869003410743282"/>
+          <c:w val="0.87202234185615335"/>
+          <c:h val="0.69944652191551782"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1535,6 +1535,7 @@
         <c:axId val="641670895"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1568,7 +1569,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx2"/>
                 </a:solidFill>
@@ -1598,8 +1599,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37461150880730126"/>
-          <c:y val="0.89459469194912034"/>
+          <c:x val="0.3653194296342116"/>
+          <c:y val="0.9000876257403424"/>
           <c:w val="0.27823225739166713"/>
           <c:h val="5.8698584306973785E-2"/>
         </c:manualLayout>
@@ -2188,8 +2189,8 @@
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>125</xdr:row>
-      <xdr:rowOff>183444</xdr:rowOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2517,10 +2518,10 @@
   <dimension ref="A1:AU118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="T45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U98" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Z61" sqref="Z61"/>
+      <selection pane="bottomRight" activeCell="Y104" sqref="Y104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4124,7 +4125,7 @@
       <c r="V19" s="10">
         <v>1751060000</v>
       </c>
-      <c r="AB19" s="66">
+      <c r="AB19" s="60">
         <f>V40-V56-V61</f>
         <v>-1165299000</v>
       </c>
@@ -8625,10 +8626,10 @@
       <c r="V83" s="1">
         <v>-104233000</v>
       </c>
-      <c r="AC83" s="59" t="s">
+      <c r="AC83" s="63" t="s">
         <v>126</v>
       </c>
-      <c r="AD83" s="60"/>
+      <c r="AD83" s="64"/>
     </row>
     <row r="84" spans="1:46" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
@@ -8695,10 +8696,10 @@
         <v>66156000</v>
       </c>
       <c r="V84" s="1"/>
-      <c r="AC84" s="61" t="s">
+      <c r="AC84" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="AD84" s="62"/>
+      <c r="AD84" s="66"/>
     </row>
     <row r="85" spans="1:46" ht="20" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
@@ -9400,10 +9401,10 @@
         <f>V88</f>
         <v>-312126000</v>
       </c>
-      <c r="AC93" s="61" t="s">
+      <c r="AC93" s="65" t="s">
         <v>134</v>
       </c>
-      <c r="AD93" s="62"/>
+      <c r="AD93" s="66"/>
     </row>
     <row r="94" spans="1:46" ht="20" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
@@ -9769,10 +9770,10 @@
       <c r="V98" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AC98" s="61" t="s">
+      <c r="AC98" s="65" t="s">
         <v>139</v>
       </c>
-      <c r="AD98" s="62"/>
+      <c r="AD98" s="66"/>
     </row>
     <row r="99" spans="1:46" ht="20" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
@@ -10215,10 +10216,10 @@
       <c r="V104" s="11">
         <v>737877000</v>
       </c>
-      <c r="AC104" s="61" t="s">
+      <c r="AC104" s="65" t="s">
         <v>145</v>
       </c>
-      <c r="AD104" s="62"/>
+      <c r="AD104" s="66"/>
     </row>
     <row r="105" spans="1:46" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
@@ -10512,10 +10513,10 @@
       </c>
     </row>
     <row r="109" spans="1:46" ht="19" x14ac:dyDescent="0.25">
-      <c r="W109" s="63" t="s">
+      <c r="W109" s="61" t="s">
         <v>151</v>
       </c>
-      <c r="X109" s="64"/>
+      <c r="X109" s="62"/>
     </row>
     <row r="110" spans="1:46" ht="20" x14ac:dyDescent="0.25">
       <c r="W110" s="50" t="s">
@@ -10557,7 +10558,7 @@
       <c r="W114" s="50" t="s">
         <v>155</v>
       </c>
-      <c r="X114" s="65">
+      <c r="X114" s="59">
         <f>V34*(1+(5*AB16))</f>
         <v>43003211.19368273</v>
       </c>

</xml_diff>